<commit_message>
[DC-1404] update date_shift notebooks
</commit_message>
<xml_diff>
--- a/data_steward/analytics/rt_cdr_qc/rt_cdr_qc_result.xlsx
+++ b/data_steward/analytics/rt_cdr_qc/rt_cdr_qc_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qianj/Documents/aou/curation/RT_notebook_final_update/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B8146E-31A5-AD4E-ADAE-C7BA5019CAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FD3A82-EF73-D745-BEDF-DDA8D0C98341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="980" windowWidth="27640" windowHeight="15860" xr2:uid="{32211158-6419-1A40-8571-3DCDE431D8DC}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15860" xr2:uid="{32211158-6419-1A40-8571-3DCDE431D8DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>R2020q4r1</t>
   </si>
@@ -88,12 +88,6 @@
   </si>
   <si>
     <t>report4_dateshift</t>
-  </si>
-  <si>
-    <t>same error in both new and old cdr</t>
-  </si>
-  <si>
-    <t>Query6 Death. DS_6 Verify that the field identified to follow the date shift rule as de-identification action in DEATH table have been randomly date shifted.</t>
   </si>
   <si>
     <t>report5_row_suppression_icd</t>
@@ -558,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E06919-C49B-6F4A-8279-5B857AD29F8C}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +574,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -589,7 +583,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="255" x14ac:dyDescent="0.2">
@@ -600,16 +594,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="187" x14ac:dyDescent="0.2">
@@ -620,16 +614,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -655,7 +649,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
@@ -664,7 +658,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -675,7 +669,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -702,19 +696,16 @@
         <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -722,19 +713,19 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="238" x14ac:dyDescent="0.2">
@@ -742,19 +733,19 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="204" x14ac:dyDescent="0.2">
@@ -762,38 +753,38 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="221" x14ac:dyDescent="0.2">
@@ -801,22 +792,22 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="136" x14ac:dyDescent="0.2">
@@ -824,22 +815,22 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>